<commit_message>
vraagsysteem werk soort van
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -23,7 +23,7 @@
     <t>punten_an</t>
   </si>
   <si>
-    <t xml:space="preserve">punten_ad </t>
+    <t>punten_ad</t>
   </si>
   <si>
     <t>punten_re</t>
@@ -41,7 +41,7 @@
     <t>uitkomst</t>
   </si>
   <si>
-    <t>joost</t>
+    <t>Joost</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,9 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s"/>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
       <c r="C2" t="s"/>
       <c r="D2" t="s"/>
       <c r="E2" t="s"/>

</xml_diff>

<commit_message>
Vraagfunctie final final final
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joost\Documents\SortingHat\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D08B1E-C4CE-4D24-AB36-CEB9B0F0A2BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="db" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="db" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>naam</t>
   </si>
@@ -39,28 +44,24 @@
   </si>
   <si>
     <t>uitkomst</t>
-  </si>
-  <si>
-    <t>Jesse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,15 +77,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -372,19 +382,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,20 +417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="s"/>
-      <c r="D2" t="s"/>
-      <c r="E2" t="s"/>
-      <c r="F2" t="s"/>
-      <c r="G2" t="s"/>
-      <c r="H2" t="s"/>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added styling to uitslag
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="db" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="db" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>naam</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>Hallo</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>yeet</t>
+  </si>
+  <si>
+    <t>wwwww</t>
   </si>
 </sst>
 </file>
@@ -437,6 +446,60 @@
       </c>
       <c r="F3" t="s"/>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>68</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>